<commit_message>
added hardware guide and stls
</commit_message>
<xml_diff>
--- a/Build Guide/sand_table_bom.xlsx
+++ b/Build Guide/sand_table_bom.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ravidudhagra/Documents/Other/Sand Table/Build Guide/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AABB7D01-8044-DC4F-ABA0-4A8377679C92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF5D5CF1-57FB-224D-A774-2C8E0A6E4706}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="20100" xr2:uid="{A342AD51-B7B9-D742-B483-2CBFB6497458}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="121">
   <si>
     <t>Sand Table Bill of Materials</t>
   </si>
@@ -441,6 +441,12 @@
   </si>
   <si>
     <t>Micro SD Card</t>
+  </si>
+  <si>
+    <t>1" Cube Neodynium Magnet</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/CMS-Magnetics-Grade-Neodymium-Magnet/dp/B008D3NXQO/ref=sr_1_12?dchild=1&amp;keywords=1+in+cube+neodymium+magnet&amp;qid=1599060210&amp;sr=8-12</t>
   </si>
 </sst>
 </file>
@@ -669,14 +675,8 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -689,9 +689,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -707,9 +704,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -725,17 +719,8 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="2" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -756,14 +741,38 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -824,6 +833,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-4565-9541-BABD-8177CD570497}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -839,6 +853,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-4565-9541-BABD-8177CD570497}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -854,6 +873,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-4565-9541-BABD-8177CD570497}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -911,7 +935,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$D$45:$D$47</c:f>
+              <c:f>Sheet1!$D$46:$D$48</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -928,7 +952,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$45:$F$47</c:f>
+              <c:f>Sheet1!$F$46:$F$48</c:f>
               <c:numCache>
                 <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="3"/>
@@ -936,7 +960,7 @@
                   <c:v>272.58999999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>408.86000000000007</c:v>
+                  <c:v>421.84000000000009</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>41.94</c:v>
@@ -1609,13 +1633,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>2836334</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>131233</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>3767667</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>264584</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1898,968 +1922,988 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="26"/>
   <cols>
-    <col min="1" max="1" width="4.83203125" style="12" customWidth="1"/>
-    <col min="2" max="2" width="40.1640625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="50.83203125" style="11" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="9"/>
-    <col min="5" max="5" width="10.83203125" style="10"/>
-    <col min="6" max="6" width="10.83203125" style="9"/>
-    <col min="7" max="7" width="50.83203125" style="8" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="6"/>
+    <col min="1" max="1" width="4.83203125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="40.1640625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="50.83203125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="6"/>
+    <col min="5" max="5" width="10.83203125" style="7"/>
+    <col min="6" max="6" width="10.83203125" style="6"/>
+    <col min="7" max="7" width="50.83203125" style="5" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="24">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" s="31" customFormat="1" ht="24">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" ht="20">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" s="4" customFormat="1" ht="17" thickBot="1">
-      <c r="A3" s="7" t="s">
+    <row r="2" spans="1:7" s="32" customFormat="1" ht="20">
+      <c r="A2" s="32" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="2" customFormat="1" ht="17" thickBot="1">
+      <c r="A3" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="5" t="s">
+      <c r="B3" s="33"/>
+      <c r="C3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="34" customHeight="1">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="25">
+      <c r="D4" s="18">
         <v>22.22</v>
       </c>
-      <c r="E4" s="26">
+      <c r="E4" s="19">
         <v>2</v>
       </c>
-      <c r="F4" s="25">
+      <c r="F4" s="18">
         <f>D4*E4</f>
         <v>44.44</v>
       </c>
-      <c r="G4" s="23" t="s">
+      <c r="G4" s="16" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="17">
-      <c r="A5" s="13"/>
-      <c r="B5" s="14" t="s">
+      <c r="A5" s="26"/>
+      <c r="B5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="11">
         <v>35.950000000000003</v>
       </c>
-      <c r="E5" s="16">
-        <v>1</v>
-      </c>
-      <c r="F5" s="15">
-        <f t="shared" ref="F5:F68" si="0">D5*E5</f>
+      <c r="E5" s="12">
+        <v>1</v>
+      </c>
+      <c r="F5" s="11">
+        <f t="shared" ref="F5:F42" si="0">D5*E5</f>
         <v>35.950000000000003</v>
       </c>
-      <c r="G5" s="14"/>
+      <c r="G5" s="10"/>
     </row>
     <row r="6" spans="1:7" ht="17">
-      <c r="A6" s="13"/>
-      <c r="B6" s="14" t="s">
+      <c r="A6" s="26"/>
+      <c r="B6" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="11">
         <v>10.48</v>
       </c>
-      <c r="E6" s="16">
-        <v>1</v>
-      </c>
-      <c r="F6" s="15">
+      <c r="E6" s="12">
+        <v>1</v>
+      </c>
+      <c r="F6" s="11">
         <f t="shared" si="0"/>
         <v>10.48</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="G6" s="10" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="17">
-      <c r="A7" s="13"/>
-      <c r="B7" s="14" t="s">
+      <c r="A7" s="26"/>
+      <c r="B7" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="11">
         <v>4.75</v>
       </c>
-      <c r="E7" s="16">
-        <v>1</v>
-      </c>
-      <c r="F7" s="15">
+      <c r="E7" s="12">
+        <v>1</v>
+      </c>
+      <c r="F7" s="11">
         <f t="shared" si="0"/>
         <v>4.75</v>
       </c>
-      <c r="G7" s="14"/>
+      <c r="G7" s="10"/>
     </row>
     <row r="8" spans="1:7" ht="17">
-      <c r="A8" s="13"/>
-      <c r="B8" s="14" t="s">
+      <c r="A8" s="26"/>
+      <c r="B8" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="11">
         <v>3.98</v>
       </c>
-      <c r="E8" s="16">
+      <c r="E8" s="12">
         <v>6</v>
       </c>
-      <c r="F8" s="15">
+      <c r="F8" s="11">
         <f t="shared" si="0"/>
         <v>23.88</v>
       </c>
-      <c r="G8" s="14" t="s">
+      <c r="G8" s="10" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="34">
-      <c r="A9" s="13"/>
-      <c r="B9" s="14" t="s">
+      <c r="A9" s="26"/>
+      <c r="B9" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="11">
         <v>3.98</v>
       </c>
-      <c r="E9" s="16">
+      <c r="E9" s="12">
         <v>4</v>
       </c>
-      <c r="F9" s="15">
+      <c r="F9" s="11">
         <f t="shared" si="0"/>
         <v>15.92</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="G9" s="10" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="34">
-      <c r="A10" s="13"/>
-      <c r="B10" s="14" t="s">
+      <c r="A10" s="26"/>
+      <c r="B10" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="11">
         <v>3.98</v>
       </c>
-      <c r="E10" s="16">
-        <v>1</v>
-      </c>
-      <c r="F10" s="15">
+      <c r="E10" s="12">
+        <v>1</v>
+      </c>
+      <c r="F10" s="11">
         <f t="shared" si="0"/>
         <v>3.98</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="G10" s="10" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="17">
-      <c r="A11" s="13"/>
-      <c r="B11" s="14" t="s">
+      <c r="A11" s="26"/>
+      <c r="B11" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="11">
         <v>2.27</v>
       </c>
-      <c r="E11" s="16">
-        <v>1</v>
-      </c>
-      <c r="F11" s="15">
+      <c r="E11" s="12">
+        <v>1</v>
+      </c>
+      <c r="F11" s="11">
         <f t="shared" si="0"/>
         <v>2.27</v>
       </c>
-      <c r="G11" s="14" t="s">
+      <c r="G11" s="10" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="34">
-      <c r="A12" s="13"/>
-      <c r="B12" s="14" t="s">
+      <c r="A12" s="26"/>
+      <c r="B12" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="11">
         <v>0.97</v>
       </c>
-      <c r="E12" s="16">
-        <v>1</v>
-      </c>
-      <c r="F12" s="15">
+      <c r="E12" s="12">
+        <v>1</v>
+      </c>
+      <c r="F12" s="11">
         <f t="shared" si="0"/>
         <v>0.97</v>
       </c>
-      <c r="G12" s="14" t="s">
+      <c r="G12" s="10" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="51">
-      <c r="A13" s="13"/>
-      <c r="B13" s="14" t="s">
+      <c r="A13" s="26"/>
+      <c r="B13" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="11">
         <v>30</v>
       </c>
-      <c r="E13" s="16">
-        <v>1</v>
-      </c>
-      <c r="F13" s="15">
+      <c r="E13" s="12">
+        <v>1</v>
+      </c>
+      <c r="F13" s="11">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="G13" s="14" t="s">
+      <c r="G13" s="10" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="51">
-      <c r="A14" s="13"/>
-      <c r="B14" s="14" t="s">
+      <c r="A14" s="26"/>
+      <c r="B14" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="D14" s="15">
+      <c r="D14" s="11">
         <v>99.95</v>
       </c>
-      <c r="E14" s="16">
-        <v>1</v>
-      </c>
-      <c r="F14" s="15">
+      <c r="E14" s="12">
+        <v>1</v>
+      </c>
+      <c r="F14" s="11">
         <f t="shared" si="0"/>
         <v>99.95</v>
       </c>
-      <c r="G14" s="14" t="s">
+      <c r="G14" s="10" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="51" customHeight="1">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="15">
+      <c r="D15" s="11">
         <v>22.99</v>
       </c>
-      <c r="E15" s="16">
-        <v>1</v>
-      </c>
-      <c r="F15" s="15">
+      <c r="E15" s="12">
+        <v>1</v>
+      </c>
+      <c r="F15" s="11">
         <f t="shared" si="0"/>
         <v>22.99</v>
       </c>
-      <c r="G15" s="14" t="s">
+      <c r="G15" s="10" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="17">
-      <c r="A16" s="19"/>
-      <c r="B16" s="14" t="s">
+      <c r="A16" s="30"/>
+      <c r="B16" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="D16" s="15">
+      <c r="D16" s="11">
         <v>13.99</v>
       </c>
-      <c r="E16" s="16">
-        <v>1</v>
-      </c>
-      <c r="F16" s="15">
+      <c r="E16" s="12">
+        <v>1</v>
+      </c>
+      <c r="F16" s="11">
         <f t="shared" si="0"/>
         <v>13.99</v>
       </c>
-      <c r="G16" s="14" t="s">
+      <c r="G16" s="10" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="17">
-      <c r="A17" s="19"/>
-      <c r="B17" s="14" t="s">
+      <c r="A17" s="30"/>
+      <c r="B17" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="D17" s="15">
+      <c r="D17" s="11">
         <v>8.09</v>
       </c>
-      <c r="E17" s="16">
-        <v>1</v>
-      </c>
-      <c r="F17" s="15">
+      <c r="E17" s="12">
+        <v>1</v>
+      </c>
+      <c r="F17" s="11">
         <f t="shared" si="0"/>
         <v>8.09</v>
       </c>
-      <c r="G17" s="14" t="s">
+      <c r="G17" s="10" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="17">
-      <c r="A18" s="19"/>
-      <c r="B18" s="14" t="s">
+      <c r="A18" s="30"/>
+      <c r="B18" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="D18" s="15">
+      <c r="D18" s="11">
         <v>13.95</v>
       </c>
-      <c r="E18" s="16">
-        <v>1</v>
-      </c>
-      <c r="F18" s="15">
+      <c r="E18" s="12">
+        <v>1</v>
+      </c>
+      <c r="F18" s="11">
         <f>D18*E18</f>
         <v>13.95</v>
       </c>
-      <c r="G18" s="14"/>
+      <c r="G18" s="10"/>
     </row>
     <row r="19" spans="1:7" ht="17">
-      <c r="A19" s="19"/>
-      <c r="B19" s="14" t="s">
+      <c r="A19" s="30"/>
+      <c r="B19" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="D19" s="15">
+      <c r="D19" s="11">
         <v>8.99</v>
       </c>
-      <c r="E19" s="16">
-        <v>1</v>
-      </c>
-      <c r="F19" s="15">
+      <c r="E19" s="12">
+        <v>1</v>
+      </c>
+      <c r="F19" s="11">
         <f t="shared" si="0"/>
         <v>8.99</v>
       </c>
-      <c r="G19" s="14"/>
+      <c r="G19" s="10"/>
     </row>
     <row r="20" spans="1:7" ht="17">
-      <c r="A20" s="19"/>
-      <c r="B20" s="14" t="s">
+      <c r="A20" s="30"/>
+      <c r="B20" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="D20" s="15">
+      <c r="D20" s="11">
         <v>29.98</v>
       </c>
-      <c r="E20" s="16">
-        <v>1</v>
-      </c>
-      <c r="F20" s="15">
+      <c r="E20" s="12">
+        <v>1</v>
+      </c>
+      <c r="F20" s="11">
         <f t="shared" si="0"/>
         <v>29.98</v>
       </c>
-      <c r="G20" s="14" t="s">
+      <c r="G20" s="10" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="17">
-      <c r="A21" s="19"/>
-      <c r="B21" s="14" t="s">
+      <c r="A21" s="30"/>
+      <c r="B21" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="C21" s="18" t="s">
+      <c r="C21" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="D21" s="15">
+      <c r="D21" s="11">
         <v>5.82</v>
       </c>
-      <c r="E21" s="16">
-        <v>1</v>
-      </c>
-      <c r="F21" s="15">
+      <c r="E21" s="12">
+        <v>1</v>
+      </c>
+      <c r="F21" s="11">
         <f t="shared" si="0"/>
         <v>5.82</v>
       </c>
-      <c r="G21" s="14" t="s">
+      <c r="G21" s="10" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="51">
-      <c r="A22" s="19"/>
-      <c r="B22" s="14" t="s">
+      <c r="A22" s="30"/>
+      <c r="B22" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="C22" s="18" t="s">
+      <c r="C22" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="D22" s="15">
+      <c r="D22" s="11">
         <v>6.98</v>
       </c>
-      <c r="E22" s="16">
-        <v>1</v>
-      </c>
-      <c r="F22" s="15">
+      <c r="E22" s="12">
+        <v>1</v>
+      </c>
+      <c r="F22" s="11">
         <f t="shared" si="0"/>
         <v>6.98</v>
       </c>
-      <c r="G22" s="14" t="s">
+      <c r="G22" s="10" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="34">
-      <c r="A23" s="19"/>
-      <c r="B23" s="14" t="s">
+      <c r="A23" s="30"/>
+      <c r="B23" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="C23" s="18" t="s">
+      <c r="C23" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="D23" s="15">
+      <c r="D23" s="11">
         <v>15.99</v>
       </c>
-      <c r="E23" s="16">
-        <v>1</v>
-      </c>
-      <c r="F23" s="15">
+      <c r="E23" s="12">
+        <v>1</v>
+      </c>
+      <c r="F23" s="11">
         <f t="shared" si="0"/>
         <v>15.99</v>
       </c>
-      <c r="G23" s="14" t="s">
+      <c r="G23" s="10" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="51">
-      <c r="A24" s="19"/>
-      <c r="B24" s="14" t="s">
+      <c r="A24" s="30"/>
+      <c r="B24" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="C24" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="D24" s="15">
+      <c r="D24" s="11">
         <v>12.99</v>
       </c>
-      <c r="E24" s="16">
+      <c r="E24" s="12">
         <v>2</v>
       </c>
-      <c r="F24" s="15">
+      <c r="F24" s="11">
         <f t="shared" si="0"/>
         <v>25.98</v>
       </c>
-      <c r="G24" s="14" t="s">
+      <c r="G24" s="10" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="17">
-      <c r="A25" s="19"/>
-      <c r="B25" s="14" t="s">
+      <c r="A25" s="30"/>
+      <c r="B25" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="C25" s="18" t="s">
+      <c r="C25" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="D25" s="15">
+      <c r="D25" s="11">
         <v>19.989999999999998</v>
       </c>
-      <c r="E25" s="16">
-        <v>1</v>
-      </c>
-      <c r="F25" s="15">
+      <c r="E25" s="12">
+        <v>1</v>
+      </c>
+      <c r="F25" s="11">
         <f t="shared" si="0"/>
         <v>19.989999999999998</v>
       </c>
-      <c r="G25" s="14"/>
+      <c r="G25" s="10"/>
     </row>
     <row r="26" spans="1:7" ht="17">
-      <c r="A26" s="19"/>
-      <c r="B26" s="14" t="s">
+      <c r="A26" s="30"/>
+      <c r="B26" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="C26" s="18" t="s">
+      <c r="C26" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="D26" s="15">
+      <c r="D26" s="11">
         <v>8.48</v>
       </c>
-      <c r="E26" s="16">
+      <c r="E26" s="12">
         <v>2</v>
       </c>
-      <c r="F26" s="15">
+      <c r="F26" s="11">
         <f t="shared" si="0"/>
         <v>16.96</v>
       </c>
-      <c r="G26" s="14"/>
+      <c r="G26" s="10"/>
     </row>
     <row r="27" spans="1:7" ht="17">
-      <c r="A27" s="19"/>
-      <c r="B27" s="14" t="s">
+      <c r="A27" s="30"/>
+      <c r="B27" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="C27" s="18" t="s">
+      <c r="C27" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="D27" s="15">
+      <c r="D27" s="11">
         <v>10.99</v>
       </c>
-      <c r="E27" s="16">
-        <v>1</v>
-      </c>
-      <c r="F27" s="15">
+      <c r="E27" s="12">
+        <v>1</v>
+      </c>
+      <c r="F27" s="11">
         <f t="shared" si="0"/>
         <v>10.99</v>
       </c>
-      <c r="G27" s="14"/>
+      <c r="G27" s="10"/>
     </row>
     <row r="28" spans="1:7" ht="17">
-      <c r="A28" s="19"/>
-      <c r="B28" s="14" t="s">
+      <c r="A28" s="30"/>
+      <c r="B28" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C28" s="18" t="s">
+      <c r="C28" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="D28" s="15">
+      <c r="D28" s="11">
         <v>9.99</v>
       </c>
-      <c r="E28" s="16">
+      <c r="E28" s="12">
         <v>2</v>
       </c>
-      <c r="F28" s="15">
+      <c r="F28" s="11">
         <f t="shared" si="0"/>
         <v>19.98</v>
       </c>
-      <c r="G28" s="14"/>
+      <c r="G28" s="10"/>
     </row>
     <row r="29" spans="1:7" ht="26" customHeight="1">
-      <c r="A29" s="19"/>
-      <c r="B29" s="14" t="s">
+      <c r="A29" s="30"/>
+      <c r="B29" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="C29" s="18" t="s">
+      <c r="C29" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="D29" s="15">
+      <c r="D29" s="11">
         <v>7.96</v>
       </c>
-      <c r="E29" s="16">
-        <v>1</v>
-      </c>
-      <c r="F29" s="15">
+      <c r="E29" s="12">
+        <v>1</v>
+      </c>
+      <c r="F29" s="11">
         <f t="shared" si="0"/>
         <v>7.96</v>
       </c>
-      <c r="G29" s="14"/>
+      <c r="G29" s="10"/>
     </row>
     <row r="30" spans="1:7" ht="26" customHeight="1">
-      <c r="A30" s="19"/>
-      <c r="B30" s="14" t="s">
+      <c r="A30" s="30"/>
+      <c r="B30" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="C30" s="18" t="s">
+      <c r="C30" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="D30" s="15">
+      <c r="D30" s="11">
         <v>12.99</v>
       </c>
-      <c r="E30" s="16">
-        <v>1</v>
-      </c>
-      <c r="F30" s="15">
+      <c r="E30" s="12">
+        <v>1</v>
+      </c>
+      <c r="F30" s="11">
         <f t="shared" si="0"/>
         <v>12.99</v>
       </c>
-      <c r="G30" s="14" t="s">
+      <c r="G30" s="10" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="51">
-      <c r="A31" s="19"/>
-      <c r="B31" s="14" t="s">
+      <c r="A31" s="30"/>
+      <c r="B31" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="C31" s="20" t="s">
+      <c r="C31" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="D31" s="15">
+      <c r="D31" s="11">
         <v>15.99</v>
       </c>
-      <c r="E31" s="16">
-        <v>1</v>
-      </c>
-      <c r="F31" s="15">
+      <c r="E31" s="12">
+        <v>1</v>
+      </c>
+      <c r="F31" s="11">
         <f t="shared" si="0"/>
         <v>15.99</v>
       </c>
-      <c r="G31" s="14" t="s">
+      <c r="G31" s="10" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="26" customHeight="1">
-      <c r="A32" s="19"/>
-      <c r="B32" s="14" t="s">
+      <c r="A32" s="30"/>
+      <c r="B32" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="C32" s="18" t="s">
+      <c r="C32" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="D32" s="15">
+      <c r="D32" s="11">
         <v>25.98</v>
       </c>
-      <c r="E32" s="16">
-        <v>1</v>
-      </c>
-      <c r="F32" s="15">
+      <c r="E32" s="12">
+        <v>1</v>
+      </c>
+      <c r="F32" s="11">
         <f t="shared" si="0"/>
         <v>25.98</v>
       </c>
-      <c r="G32" s="14" t="s">
+      <c r="G32" s="10" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="26" customHeight="1">
-      <c r="A33" s="19"/>
-      <c r="B33" s="14" t="s">
+      <c r="A33" s="30"/>
+      <c r="B33" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="C33" s="18" t="s">
+      <c r="C33" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="D33" s="15">
+      <c r="D33" s="11">
         <v>3.66</v>
       </c>
-      <c r="E33" s="16">
-        <v>1</v>
-      </c>
-      <c r="F33" s="15">
+      <c r="E33" s="12">
+        <v>1</v>
+      </c>
+      <c r="F33" s="11">
         <f t="shared" si="0"/>
         <v>3.66</v>
       </c>
-      <c r="G33" s="14"/>
+      <c r="G33" s="10"/>
     </row>
     <row r="34" spans="1:7" ht="26" customHeight="1">
-      <c r="A34" s="19"/>
-      <c r="B34" s="14" t="s">
+      <c r="A34" s="30"/>
+      <c r="B34" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="C34" s="18" t="s">
+      <c r="C34" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="D34" s="15">
+      <c r="D34" s="11">
         <v>5.64</v>
       </c>
-      <c r="E34" s="16">
-        <v>1</v>
-      </c>
-      <c r="F34" s="15">
+      <c r="E34" s="12">
+        <v>1</v>
+      </c>
+      <c r="F34" s="11">
         <f t="shared" si="0"/>
         <v>5.64</v>
       </c>
-      <c r="G34" s="14"/>
+      <c r="G34" s="10"/>
     </row>
     <row r="35" spans="1:7" ht="34">
-      <c r="A35" s="19"/>
-      <c r="B35" s="14" t="s">
+      <c r="A35" s="30"/>
+      <c r="B35" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="C35" s="18" t="s">
+      <c r="C35" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="D35" s="15">
+      <c r="D35" s="11">
         <v>30</v>
       </c>
-      <c r="E35" s="16">
-        <v>1</v>
-      </c>
-      <c r="F35" s="15">
+      <c r="E35" s="12">
+        <v>1</v>
+      </c>
+      <c r="F35" s="11">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="G35" s="14" t="s">
+      <c r="G35" s="10" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="26" customHeight="1">
-      <c r="A36" s="19"/>
-      <c r="B36" s="14" t="s">
+      <c r="A36" s="30"/>
+      <c r="B36" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="C36" s="18" t="s">
+      <c r="C36" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="D36" s="15">
+      <c r="D36" s="11">
         <v>6.19</v>
       </c>
-      <c r="E36" s="16">
-        <v>1</v>
-      </c>
-      <c r="F36" s="15">
+      <c r="E36" s="12">
+        <v>1</v>
+      </c>
+      <c r="F36" s="11">
         <f t="shared" si="0"/>
         <v>6.19</v>
       </c>
-      <c r="G36" s="14" t="s">
+      <c r="G36" s="10" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="85">
-      <c r="A37" s="19"/>
-      <c r="B37" s="14" t="s">
+      <c r="A37" s="30"/>
+      <c r="B37" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="C37" s="18" t="s">
+      <c r="C37" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="D37" s="15">
+      <c r="D37" s="11">
         <v>24.99</v>
       </c>
-      <c r="E37" s="16">
-        <v>1</v>
-      </c>
-      <c r="F37" s="15">
+      <c r="E37" s="12">
+        <v>1</v>
+      </c>
+      <c r="F37" s="11">
         <f t="shared" si="0"/>
         <v>24.99</v>
       </c>
-      <c r="G37" s="14" t="s">
+      <c r="G37" s="10" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="51">
-      <c r="A38" s="19"/>
-      <c r="B38" s="14" t="s">
+      <c r="A38" s="30"/>
+      <c r="B38" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="C38" s="18" t="s">
+      <c r="C38" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="D38" s="15">
+      <c r="D38" s="11">
         <v>20.9</v>
       </c>
-      <c r="E38" s="16">
+      <c r="E38" s="12">
         <v>2</v>
       </c>
-      <c r="F38" s="15">
+      <c r="F38" s="11">
         <f t="shared" si="0"/>
         <v>41.8</v>
       </c>
-      <c r="G38" s="14" t="s">
+      <c r="G38" s="10" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="34">
-      <c r="A39" s="19"/>
-      <c r="B39" s="14" t="s">
+    <row r="39" spans="1:7" ht="17">
+      <c r="A39" s="30"/>
+      <c r="B39" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="D39" s="21">
+        <v>12.98</v>
+      </c>
+      <c r="E39" s="12">
+        <v>1</v>
+      </c>
+      <c r="F39" s="21">
+        <f t="shared" si="0"/>
+        <v>12.98</v>
+      </c>
+      <c r="G39" s="10"/>
+    </row>
+    <row r="40" spans="1:7" ht="34">
+      <c r="A40" s="30"/>
+      <c r="B40" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="C39" s="18" t="s">
+      <c r="C40" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="D39" s="15">
+      <c r="D40" s="11">
         <v>12.98</v>
       </c>
-      <c r="E39" s="16">
-        <v>1</v>
-      </c>
-      <c r="F39" s="15">
+      <c r="E40" s="12">
+        <v>1</v>
+      </c>
+      <c r="F40" s="11">
         <f t="shared" si="0"/>
         <v>12.98</v>
       </c>
-      <c r="G39" s="14" t="s">
+      <c r="G40" s="10" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="34">
-      <c r="A40" s="21" t="s">
+    <row r="41" spans="1:7" ht="34">
+      <c r="A41" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="B40" s="14" t="s">
+      <c r="B41" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="C40" s="18" t="s">
+      <c r="C41" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="D40" s="15">
+      <c r="D41" s="11">
         <v>14.99</v>
       </c>
-      <c r="E40" s="16">
+      <c r="E41" s="12">
         <v>2</v>
       </c>
-      <c r="F40" s="15">
+      <c r="F41" s="11">
         <f t="shared" si="0"/>
         <v>29.98</v>
       </c>
-      <c r="G40" s="14" t="s">
+      <c r="G41" s="10" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="26" customHeight="1">
-      <c r="A41" s="21"/>
-      <c r="B41" s="14" t="s">
+    <row r="42" spans="1:7" ht="26" customHeight="1">
+      <c r="A42" s="24"/>
+      <c r="B42" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="C41" s="18" t="s">
+      <c r="C42" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="D41" s="15">
+      <c r="D42" s="11">
         <v>5.99</v>
       </c>
-      <c r="E41" s="16">
-        <v>1</v>
-      </c>
-      <c r="F41" s="15">
+      <c r="E42" s="12">
+        <v>1</v>
+      </c>
+      <c r="F42" s="11">
         <f t="shared" si="0"/>
         <v>5.99</v>
       </c>
-      <c r="G41" s="14" t="s">
+      <c r="G42" s="10" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="17">
-      <c r="A42" s="21"/>
-      <c r="B42" s="14" t="s">
+    <row r="43" spans="1:7" ht="17">
+      <c r="A43" s="24"/>
+      <c r="B43" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C42" s="18" t="s">
+      <c r="C43" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D42" s="15">
+      <c r="D43" s="11">
         <v>5.97</v>
       </c>
-      <c r="E42" s="16">
-        <v>1</v>
-      </c>
-      <c r="F42" s="15">
-        <f>D42*E42</f>
+      <c r="E43" s="12">
+        <v>1</v>
+      </c>
+      <c r="F43" s="11">
+        <f>D43*E43</f>
         <v>5.97</v>
       </c>
-      <c r="G42" s="14" t="s">
+      <c r="G43" s="10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
-      <c r="C43" s="27"/>
-    </row>
     <row r="44" spans="1:7">
-      <c r="C44" s="27"/>
+      <c r="C44" s="20"/>
     </row>
     <row r="45" spans="1:7">
-      <c r="C45" s="27"/>
-      <c r="D45" s="28" t="s">
+      <c r="C45" s="20"/>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="C46" s="20"/>
+      <c r="D46" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="E45" s="28"/>
-      <c r="F45" s="15">
+      <c r="E46" s="27"/>
+      <c r="F46" s="11">
         <f>SUM(F4:F14)</f>
         <v>272.58999999999997</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
-      <c r="C46" s="27"/>
-      <c r="D46" s="28" t="s">
+    <row r="47" spans="1:7">
+      <c r="C47" s="20"/>
+      <c r="D47" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="E46" s="28"/>
-      <c r="F46" s="15">
-        <f>SUM(F15:F39)</f>
-        <v>408.86000000000007</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="27" thickBot="1">
-      <c r="C47" s="27"/>
-      <c r="D47" s="29" t="s">
+      <c r="E47" s="27"/>
+      <c r="F47" s="11">
+        <f>SUM(F15:F40)</f>
+        <v>421.84000000000009</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="27" thickBot="1">
+      <c r="C48" s="20"/>
+      <c r="D48" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="E47" s="29"/>
-      <c r="F47" s="30">
-        <f>SUM(F40:F42)</f>
+      <c r="E48" s="28"/>
+      <c r="F48" s="22">
+        <f>SUM(F41:F43)</f>
         <v>41.94</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
-      <c r="C48" s="27"/>
-      <c r="D48" s="31" t="s">
+    <row r="49" spans="3:6">
+      <c r="C49" s="20"/>
+      <c r="D49" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="E48" s="31"/>
-      <c r="F48" s="32">
-        <f>SUM(F4:F42)</f>
-        <v>723.3900000000001</v>
-      </c>
-    </row>
-    <row r="49" spans="3:3">
-      <c r="C49" s="27"/>
-    </row>
-    <row r="50" spans="3:3">
-      <c r="C50" s="27"/>
-    </row>
-    <row r="51" spans="3:3">
-      <c r="C51" s="27"/>
+      <c r="E49" s="29"/>
+      <c r="F49" s="23">
+        <f>SUM(F4:F43)</f>
+        <v>736.37000000000012</v>
+      </c>
+    </row>
+    <row r="50" spans="3:6">
+      <c r="C50" s="20"/>
+    </row>
+    <row r="51" spans="3:6">
+      <c r="C51" s="20"/>
+    </row>
+    <row r="52" spans="3:6">
+      <c r="C52" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="A40:A42"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="A15:A40"/>
+    <mergeCell ref="A1:XFD1"/>
+    <mergeCell ref="A2:XFD2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A41:A43"/>
     <mergeCell ref="A4:A14"/>
-    <mergeCell ref="D45:E45"/>
     <mergeCell ref="D46:E46"/>
     <mergeCell ref="D47:E47"/>
     <mergeCell ref="D48:E48"/>
-    <mergeCell ref="A15:A39"/>
-    <mergeCell ref="A1:XFD1"/>
-    <mergeCell ref="A2:XFD2"/>
-    <mergeCell ref="A3:B3"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Added M5 10mm bolts to BOM
For some reason they weren't there before, so that should be fixed now
</commit_message>
<xml_diff>
--- a/Build Guide/sand_table_bom.xlsx
+++ b/Build Guide/sand_table_bom.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ravidudhagra/Documents/Other/Sand Table/Build Guide/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF5D5CF1-57FB-224D-A774-2C8E0A6E4706}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B42EDF1-F9FC-BB40-8BA2-A1DB640B3330}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="20100" xr2:uid="{A342AD51-B7B9-D742-B483-2CBFB6497458}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="123">
   <si>
     <t>Sand Table Bill of Materials</t>
   </si>
@@ -448,6 +448,12 @@
   <si>
     <t>https://www.amazon.com/CMS-Magnetics-Grade-Neodymium-Magnet/dp/B008D3NXQO/ref=sr_1_12?dchild=1&amp;keywords=1+in+cube+neodymium+magnet&amp;qid=1599060210&amp;sr=8-12</t>
   </si>
+  <si>
+    <t>M5 10mm bolts</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B07KWQ4JFK/ref=ppx_yo_dt_b_search_asin_title?ie=UTF8&amp;psc=1</t>
+  </si>
 </sst>
 </file>
 
@@ -456,7 +462,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -713,19 +719,12 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="2" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -744,6 +743,24 @@
     <xf numFmtId="44" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="6" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -759,20 +776,9 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="6" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -935,7 +941,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$D$46:$D$48</c:f>
+              <c:f>Sheet1!$D$47:$D$49</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -952,7 +958,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$46:$F$48</c:f>
+              <c:f>Sheet1!$F$47:$F$49</c:f>
               <c:numCache>
                 <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="3"/>
@@ -960,7 +966,7 @@
                   <c:v>272.58999999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>421.84000000000009</c:v>
+                  <c:v>430.3300000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>41.94</c:v>
@@ -1633,13 +1639,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>2836334</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>131233</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>3767667</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>264584</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1922,13 +1928,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G52"/>
+  <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="26"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.83203125" style="9" customWidth="1"/>
     <col min="2" max="2" width="40.1640625" style="5" customWidth="1"/>
@@ -1940,21 +1946,21 @@
     <col min="8" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="31" customFormat="1" ht="24">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:7" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="32" customFormat="1" ht="20">
-      <c r="A2" s="32" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" s="2" customFormat="1" ht="17" thickBot="1">
-      <c r="A3" s="33" t="s">
+    <row r="2" spans="1:7" s="25" customFormat="1" ht="20" x14ac:dyDescent="0.2">
+      <c r="A2" s="25" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="2" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="33"/>
+      <c r="B3" s="26"/>
       <c r="C3" s="3" t="s">
         <v>3</v>
       </c>
@@ -1971,36 +1977,36 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="34" customHeight="1">
-      <c r="A4" s="25" t="s">
+    <row r="4" spans="1:7" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="15">
         <v>22.22</v>
       </c>
-      <c r="E4" s="19">
+      <c r="E4" s="16">
         <v>2</v>
       </c>
-      <c r="F4" s="18">
+      <c r="F4" s="15">
         <f>D4*E4</f>
         <v>44.44</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="G4" s="14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="17">
-      <c r="A5" s="26"/>
+    <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="29"/>
       <c r="B5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="33" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="11">
@@ -2010,17 +2016,17 @@
         <v>1</v>
       </c>
       <c r="F5" s="11">
-        <f t="shared" ref="F5:F42" si="0">D5*E5</f>
+        <f t="shared" ref="F5:F43" si="0">D5*E5</f>
         <v>35.950000000000003</v>
       </c>
       <c r="G5" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="17">
-      <c r="A6" s="26"/>
+    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="29"/>
       <c r="B6" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="13" t="s">
         <v>15</v>
       </c>
       <c r="D6" s="11">
@@ -2037,12 +2043,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="17">
-      <c r="A7" s="26"/>
+    <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="29"/>
       <c r="B7" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="13" t="s">
         <v>18</v>
       </c>
       <c r="D7" s="11">
@@ -2057,12 +2063,12 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="17">
-      <c r="A8" s="26"/>
+    <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="29"/>
       <c r="B8" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="13" t="s">
         <v>23</v>
       </c>
       <c r="D8" s="11">
@@ -2079,12 +2085,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="34">
-      <c r="A9" s="26"/>
+    <row r="9" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A9" s="29"/>
       <c r="B9" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="13" t="s">
         <v>27</v>
       </c>
       <c r="D9" s="11">
@@ -2101,12 +2107,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="34">
-      <c r="A10" s="26"/>
+    <row r="10" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" s="29"/>
       <c r="B10" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="13" t="s">
         <v>30</v>
       </c>
       <c r="D10" s="11">
@@ -2123,12 +2129,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="17">
-      <c r="A11" s="26"/>
+    <row r="11" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="29"/>
       <c r="B11" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="13" t="s">
         <v>36</v>
       </c>
       <c r="D11" s="11">
@@ -2145,12 +2151,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="34">
-      <c r="A12" s="26"/>
+    <row r="12" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" s="29"/>
       <c r="B12" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="13" t="s">
         <v>39</v>
       </c>
       <c r="D12" s="11">
@@ -2167,12 +2173,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="51">
-      <c r="A13" s="26"/>
+    <row r="13" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A13" s="29"/>
       <c r="B13" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="13" t="s">
         <v>32</v>
       </c>
       <c r="D13" s="11">
@@ -2189,12 +2195,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="51">
-      <c r="A14" s="26"/>
+    <row r="14" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A14" s="29"/>
       <c r="B14" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="13" t="s">
         <v>42</v>
       </c>
       <c r="D14" s="11">
@@ -2211,14 +2217,14 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="51" customHeight="1">
-      <c r="A15" s="30" t="s">
+    <row r="15" spans="1:7" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="23" t="s">
         <v>44</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="13" t="s">
         <v>46</v>
       </c>
       <c r="D15" s="11">
@@ -2235,12 +2241,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="17">
-      <c r="A16" s="30"/>
+    <row r="16" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="23"/>
       <c r="B16" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="13" t="s">
         <v>49</v>
       </c>
       <c r="D16" s="11">
@@ -2257,12 +2263,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="17">
-      <c r="A17" s="30"/>
+    <row r="17" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="23"/>
       <c r="B17" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="13" t="s">
         <v>51</v>
       </c>
       <c r="D17" s="11">
@@ -2279,12 +2285,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="17">
-      <c r="A18" s="30"/>
+    <row r="18" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="23"/>
       <c r="B18" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="13" t="s">
         <v>55</v>
       </c>
       <c r="D18" s="11">
@@ -2299,618 +2305,678 @@
       </c>
       <c r="G18" s="10"/>
     </row>
-    <row r="19" spans="1:7" ht="17">
-      <c r="A19" s="30"/>
+    <row r="19" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="23"/>
       <c r="B19" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="D19" s="21">
+        <v>8.49</v>
+      </c>
+      <c r="E19" s="12">
+        <v>1</v>
+      </c>
+      <c r="F19" s="21">
+        <f>D19*E19</f>
+        <v>8.49</v>
+      </c>
+      <c r="G19" s="10"/>
+    </row>
+    <row r="20" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="23"/>
+      <c r="B20" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C20" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="D19" s="11">
+      <c r="D20" s="11">
         <v>8.99</v>
       </c>
-      <c r="E19" s="12">
-        <v>1</v>
-      </c>
-      <c r="F19" s="11">
+      <c r="E20" s="12">
+        <v>1</v>
+      </c>
+      <c r="F20" s="11">
         <f t="shared" si="0"/>
         <v>8.99</v>
       </c>
-      <c r="G19" s="10"/>
-    </row>
-    <row r="20" spans="1:7" ht="17">
-      <c r="A20" s="30"/>
-      <c r="B20" s="10" t="s">
+      <c r="G20" s="10"/>
+    </row>
+    <row r="21" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="23"/>
+      <c r="B21" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C21" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="D20" s="11">
+      <c r="D21" s="11">
         <v>29.98</v>
       </c>
-      <c r="E20" s="12">
-        <v>1</v>
-      </c>
-      <c r="F20" s="11">
+      <c r="E21" s="12">
+        <v>1</v>
+      </c>
+      <c r="F21" s="11">
         <f t="shared" si="0"/>
         <v>29.98</v>
       </c>
-      <c r="G20" s="10" t="s">
+      <c r="G21" s="10" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="17">
-      <c r="A21" s="30"/>
-      <c r="B21" s="10" t="s">
+    <row r="22" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="23"/>
+      <c r="B22" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C22" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="D21" s="11">
+      <c r="D22" s="11">
         <v>5.82</v>
       </c>
-      <c r="E21" s="12">
-        <v>1</v>
-      </c>
-      <c r="F21" s="11">
+      <c r="E22" s="12">
+        <v>1</v>
+      </c>
+      <c r="F22" s="11">
         <f t="shared" si="0"/>
         <v>5.82</v>
       </c>
-      <c r="G21" s="10" t="s">
+      <c r="G22" s="10" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="51">
-      <c r="A22" s="30"/>
-      <c r="B22" s="10" t="s">
+    <row r="23" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A23" s="23"/>
+      <c r="B23" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C23" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="D22" s="11">
+      <c r="D23" s="11">
         <v>6.98</v>
       </c>
-      <c r="E22" s="12">
-        <v>1</v>
-      </c>
-      <c r="F22" s="11">
+      <c r="E23" s="12">
+        <v>1</v>
+      </c>
+      <c r="F23" s="11">
         <f t="shared" si="0"/>
         <v>6.98</v>
       </c>
-      <c r="G22" s="10" t="s">
+      <c r="G23" s="10" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="34">
-      <c r="A23" s="30"/>
-      <c r="B23" s="10" t="s">
+    <row r="24" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A24" s="23"/>
+      <c r="B24" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C24" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="D23" s="11">
+      <c r="D24" s="11">
         <v>15.99</v>
       </c>
-      <c r="E23" s="12">
-        <v>1</v>
-      </c>
-      <c r="F23" s="11">
+      <c r="E24" s="12">
+        <v>1</v>
+      </c>
+      <c r="F24" s="11">
         <f t="shared" si="0"/>
         <v>15.99</v>
       </c>
-      <c r="G23" s="10" t="s">
+      <c r="G24" s="10" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="51">
-      <c r="A24" s="30"/>
-      <c r="B24" s="10" t="s">
+    <row r="25" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A25" s="23"/>
+      <c r="B25" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C25" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="D24" s="11">
+      <c r="D25" s="11">
         <v>12.99</v>
       </c>
-      <c r="E24" s="12">
+      <c r="E25" s="12">
         <v>2</v>
       </c>
-      <c r="F24" s="11">
+      <c r="F25" s="11">
         <f t="shared" si="0"/>
         <v>25.98</v>
       </c>
-      <c r="G24" s="10" t="s">
+      <c r="G25" s="10" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="17">
-      <c r="A25" s="30"/>
-      <c r="B25" s="10" t="s">
+    <row r="26" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="23"/>
+      <c r="B26" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C26" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="D25" s="11">
+      <c r="D26" s="11">
         <v>19.989999999999998</v>
       </c>
-      <c r="E25" s="12">
-        <v>1</v>
-      </c>
-      <c r="F25" s="11">
+      <c r="E26" s="12">
+        <v>1</v>
+      </c>
+      <c r="F26" s="11">
         <f t="shared" si="0"/>
         <v>19.989999999999998</v>
       </c>
-      <c r="G25" s="10"/>
-    </row>
-    <row r="26" spans="1:7" ht="17">
-      <c r="A26" s="30"/>
-      <c r="B26" s="10" t="s">
+      <c r="G26" s="10"/>
+    </row>
+    <row r="27" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="23"/>
+      <c r="B27" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C27" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="D26" s="11">
+      <c r="D27" s="11">
         <v>8.48</v>
       </c>
-      <c r="E26" s="12">
+      <c r="E27" s="12">
         <v>2</v>
       </c>
-      <c r="F26" s="11">
+      <c r="F27" s="11">
         <f t="shared" si="0"/>
         <v>16.96</v>
       </c>
-      <c r="G26" s="10"/>
-    </row>
-    <row r="27" spans="1:7" ht="17">
-      <c r="A27" s="30"/>
-      <c r="B27" s="10" t="s">
+      <c r="G27" s="10"/>
+    </row>
+    <row r="28" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="23"/>
+      <c r="B28" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C28" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="D27" s="11">
+      <c r="D28" s="11">
         <v>10.99</v>
       </c>
-      <c r="E27" s="12">
-        <v>1</v>
-      </c>
-      <c r="F27" s="11">
+      <c r="E28" s="12">
+        <v>1</v>
+      </c>
+      <c r="F28" s="11">
         <f t="shared" si="0"/>
         <v>10.99</v>
       </c>
-      <c r="G27" s="10"/>
-    </row>
-    <row r="28" spans="1:7" ht="17">
-      <c r="A28" s="30"/>
-      <c r="B28" s="10" t="s">
+      <c r="G28" s="10"/>
+    </row>
+    <row r="29" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="23"/>
+      <c r="B29" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="C29" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="D28" s="11">
+      <c r="D29" s="11">
         <v>9.99</v>
       </c>
-      <c r="E28" s="12">
+      <c r="E29" s="12">
         <v>2</v>
       </c>
-      <c r="F28" s="11">
+      <c r="F29" s="11">
         <f t="shared" si="0"/>
         <v>19.98</v>
       </c>
-      <c r="G28" s="10"/>
-    </row>
-    <row r="29" spans="1:7" ht="26" customHeight="1">
-      <c r="A29" s="30"/>
-      <c r="B29" s="10" t="s">
+      <c r="G29" s="10"/>
+    </row>
+    <row r="30" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="23"/>
+      <c r="B30" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="C30" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="D29" s="11">
+      <c r="D30" s="11">
         <v>7.96</v>
       </c>
-      <c r="E29" s="12">
-        <v>1</v>
-      </c>
-      <c r="F29" s="11">
+      <c r="E30" s="12">
+        <v>1</v>
+      </c>
+      <c r="F30" s="11">
         <f t="shared" si="0"/>
         <v>7.96</v>
       </c>
-      <c r="G29" s="10"/>
-    </row>
-    <row r="30" spans="1:7" ht="26" customHeight="1">
-      <c r="A30" s="30"/>
-      <c r="B30" s="10" t="s">
+      <c r="G30" s="10"/>
+    </row>
+    <row r="31" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="23"/>
+      <c r="B31" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="C30" s="14" t="s">
+      <c r="C31" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="D30" s="11">
+      <c r="D31" s="11">
         <v>12.99</v>
       </c>
-      <c r="E30" s="12">
-        <v>1</v>
-      </c>
-      <c r="F30" s="11">
+      <c r="E31" s="12">
+        <v>1</v>
+      </c>
+      <c r="F31" s="11">
         <f t="shared" si="0"/>
         <v>12.99</v>
       </c>
-      <c r="G30" s="10" t="s">
+      <c r="G31" s="10" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="51">
-      <c r="A31" s="30"/>
-      <c r="B31" s="10" t="s">
+    <row r="32" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A32" s="23"/>
+      <c r="B32" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="C31" s="15" t="s">
+      <c r="C32" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="D31" s="11">
+      <c r="D32" s="11">
         <v>15.99</v>
       </c>
-      <c r="E31" s="12">
-        <v>1</v>
-      </c>
-      <c r="F31" s="11">
+      <c r="E32" s="12">
+        <v>1</v>
+      </c>
+      <c r="F32" s="11">
         <f t="shared" si="0"/>
         <v>15.99</v>
       </c>
-      <c r="G31" s="10" t="s">
+      <c r="G32" s="10" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="26" customHeight="1">
-      <c r="A32" s="30"/>
-      <c r="B32" s="10" t="s">
+    <row r="33" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="23"/>
+      <c r="B33" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="C33" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="D32" s="11">
+      <c r="D33" s="11">
         <v>25.98</v>
       </c>
-      <c r="E32" s="12">
-        <v>1</v>
-      </c>
-      <c r="F32" s="11">
+      <c r="E33" s="12">
+        <v>1</v>
+      </c>
+      <c r="F33" s="11">
         <f t="shared" si="0"/>
         <v>25.98</v>
       </c>
-      <c r="G32" s="10" t="s">
+      <c r="G33" s="10" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="26" customHeight="1">
-      <c r="A33" s="30"/>
-      <c r="B33" s="10" t="s">
+    <row r="34" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="23"/>
+      <c r="B34" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="C33" s="14" t="s">
+      <c r="C34" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="D33" s="11">
+      <c r="D34" s="11">
         <v>3.66</v>
       </c>
-      <c r="E33" s="12">
-        <v>1</v>
-      </c>
-      <c r="F33" s="11">
+      <c r="E34" s="12">
+        <v>1</v>
+      </c>
+      <c r="F34" s="11">
         <f t="shared" si="0"/>
         <v>3.66</v>
       </c>
-      <c r="G33" s="10"/>
-    </row>
-    <row r="34" spans="1:7" ht="26" customHeight="1">
-      <c r="A34" s="30"/>
-      <c r="B34" s="10" t="s">
+      <c r="G34" s="10"/>
+    </row>
+    <row r="35" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="23"/>
+      <c r="B35" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="C34" s="14" t="s">
+      <c r="C35" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="D34" s="11">
+      <c r="D35" s="11">
         <v>5.64</v>
       </c>
-      <c r="E34" s="12">
-        <v>1</v>
-      </c>
-      <c r="F34" s="11">
+      <c r="E35" s="12">
+        <v>1</v>
+      </c>
+      <c r="F35" s="11">
         <f t="shared" si="0"/>
         <v>5.64</v>
       </c>
-      <c r="G34" s="10"/>
-    </row>
-    <row r="35" spans="1:7" ht="34">
-      <c r="A35" s="30"/>
-      <c r="B35" s="10" t="s">
+      <c r="G35" s="10"/>
+    </row>
+    <row r="36" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A36" s="23"/>
+      <c r="B36" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="C35" s="14" t="s">
+      <c r="C36" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="D35" s="11">
+      <c r="D36" s="11">
         <v>30</v>
       </c>
-      <c r="E35" s="12">
-        <v>1</v>
-      </c>
-      <c r="F35" s="11">
+      <c r="E36" s="12">
+        <v>1</v>
+      </c>
+      <c r="F36" s="11">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="G35" s="10" t="s">
+      <c r="G36" s="10" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="26" customHeight="1">
-      <c r="A36" s="30"/>
-      <c r="B36" s="10" t="s">
+    <row r="37" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="23"/>
+      <c r="B37" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="C36" s="14" t="s">
+      <c r="C37" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="D36" s="11">
+      <c r="D37" s="11">
         <v>6.19</v>
       </c>
-      <c r="E36" s="12">
-        <v>1</v>
-      </c>
-      <c r="F36" s="11">
+      <c r="E37" s="12">
+        <v>1</v>
+      </c>
+      <c r="F37" s="11">
         <f t="shared" si="0"/>
         <v>6.19</v>
       </c>
-      <c r="G36" s="10" t="s">
+      <c r="G37" s="10" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="85">
-      <c r="A37" s="30"/>
-      <c r="B37" s="10" t="s">
+    <row r="38" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+      <c r="A38" s="23"/>
+      <c r="B38" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="C37" s="14" t="s">
+      <c r="C38" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="D37" s="11">
+      <c r="D38" s="11">
         <v>24.99</v>
       </c>
-      <c r="E37" s="12">
-        <v>1</v>
-      </c>
-      <c r="F37" s="11">
+      <c r="E38" s="12">
+        <v>1</v>
+      </c>
+      <c r="F38" s="11">
         <f t="shared" si="0"/>
         <v>24.99</v>
       </c>
-      <c r="G37" s="10" t="s">
+      <c r="G38" s="10" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="51">
-      <c r="A38" s="30"/>
-      <c r="B38" s="10" t="s">
+    <row r="39" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A39" s="23"/>
+      <c r="B39" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="C38" s="14" t="s">
+      <c r="C39" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="D38" s="11">
+      <c r="D39" s="11">
         <v>20.9</v>
       </c>
-      <c r="E38" s="12">
+      <c r="E39" s="12">
         <v>2</v>
       </c>
-      <c r="F38" s="11">
+      <c r="F39" s="11">
         <f t="shared" si="0"/>
         <v>41.8</v>
       </c>
-      <c r="G38" s="10" t="s">
+      <c r="G39" s="10" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="17">
-      <c r="A39" s="30"/>
-      <c r="B39" s="10" t="s">
+    <row r="40" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A40" s="23"/>
+      <c r="B40" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="C39" s="14" t="s">
+      <c r="C40" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="D39" s="21">
+      <c r="D40" s="18">
         <v>12.98</v>
       </c>
-      <c r="E39" s="12">
-        <v>1</v>
-      </c>
-      <c r="F39" s="21">
+      <c r="E40" s="12">
+        <v>1</v>
+      </c>
+      <c r="F40" s="18">
         <f t="shared" si="0"/>
         <v>12.98</v>
       </c>
-      <c r="G39" s="10"/>
-    </row>
-    <row r="40" spans="1:7" ht="34">
-      <c r="A40" s="30"/>
-      <c r="B40" s="10" t="s">
+      <c r="G40" s="10"/>
+    </row>
+    <row r="41" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A41" s="23"/>
+      <c r="B41" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="C40" s="14" t="s">
+      <c r="C41" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="D40" s="11">
+      <c r="D41" s="11">
         <v>12.98</v>
       </c>
-      <c r="E40" s="12">
-        <v>1</v>
-      </c>
-      <c r="F40" s="11">
+      <c r="E41" s="12">
+        <v>1</v>
+      </c>
+      <c r="F41" s="11">
         <f t="shared" si="0"/>
         <v>12.98</v>
       </c>
-      <c r="G40" s="10" t="s">
+      <c r="G41" s="10" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="34">
-      <c r="A41" s="24" t="s">
+    <row r="42" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A42" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="B41" s="10" t="s">
+      <c r="B42" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="C41" s="14" t="s">
+      <c r="C42" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="D41" s="11">
+      <c r="D42" s="11">
         <v>14.99</v>
       </c>
-      <c r="E41" s="12">
+      <c r="E42" s="12">
         <v>2</v>
       </c>
-      <c r="F41" s="11">
+      <c r="F42" s="11">
         <f t="shared" si="0"/>
         <v>29.98</v>
       </c>
-      <c r="G41" s="10" t="s">
+      <c r="G42" s="10" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="26" customHeight="1">
-      <c r="A42" s="24"/>
-      <c r="B42" s="10" t="s">
+    <row r="43" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="27"/>
+      <c r="B43" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="C42" s="14" t="s">
+      <c r="C43" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="D42" s="11">
+      <c r="D43" s="11">
         <v>5.99</v>
       </c>
-      <c r="E42" s="12">
-        <v>1</v>
-      </c>
-      <c r="F42" s="11">
+      <c r="E43" s="12">
+        <v>1</v>
+      </c>
+      <c r="F43" s="11">
         <f t="shared" si="0"/>
         <v>5.99</v>
       </c>
-      <c r="G42" s="10" t="s">
+      <c r="G43" s="10" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="17">
-      <c r="A43" s="24"/>
-      <c r="B43" s="10" t="s">
+    <row r="44" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A44" s="27"/>
+      <c r="B44" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C43" s="14" t="s">
+      <c r="C44" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D43" s="11">
+      <c r="D44" s="11">
         <v>5.97</v>
       </c>
-      <c r="E43" s="12">
-        <v>1</v>
-      </c>
-      <c r="F43" s="11">
-        <f>D43*E43</f>
+      <c r="E44" s="12">
+        <v>1</v>
+      </c>
+      <c r="F44" s="11">
+        <f>D44*E44</f>
         <v>5.97</v>
       </c>
-      <c r="G43" s="10" t="s">
+      <c r="G44" s="10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
-      <c r="C44" s="20"/>
-    </row>
-    <row r="45" spans="1:7">
-      <c r="C45" s="20"/>
-    </row>
-    <row r="46" spans="1:7">
-      <c r="C46" s="20"/>
-      <c r="D46" s="27" t="s">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C45" s="17"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C46" s="17"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C47" s="17"/>
+      <c r="D47" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="E46" s="27"/>
-      <c r="F46" s="11">
+      <c r="E47" s="30"/>
+      <c r="F47" s="11">
         <f>SUM(F4:F14)</f>
         <v>272.58999999999997</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
-      <c r="C47" s="20"/>
-      <c r="D47" s="27" t="s">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C48" s="17"/>
+      <c r="D48" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="E47" s="27"/>
-      <c r="F47" s="11">
-        <f>SUM(F15:F40)</f>
-        <v>421.84000000000009</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="27" thickBot="1">
-      <c r="C48" s="20"/>
-      <c r="D48" s="28" t="s">
+      <c r="E48" s="30"/>
+      <c r="F48" s="11">
+        <f>SUM(F15:F41)</f>
+        <v>430.3300000000001</v>
+      </c>
+    </row>
+    <row r="49" spans="3:6" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C49" s="17"/>
+      <c r="D49" s="31" t="s">
         <v>117</v>
       </c>
-      <c r="E48" s="28"/>
-      <c r="F48" s="22">
-        <f>SUM(F41:F43)</f>
+      <c r="E49" s="31"/>
+      <c r="F49" s="19">
+        <f>SUM(F42:F44)</f>
         <v>41.94</v>
       </c>
     </row>
-    <row r="49" spans="3:6">
-      <c r="C49" s="20"/>
-      <c r="D49" s="29" t="s">
+    <row r="50" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C50" s="17"/>
+      <c r="D50" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E49" s="29"/>
-      <c r="F49" s="23">
-        <f>SUM(F4:F43)</f>
-        <v>736.37000000000012</v>
-      </c>
-    </row>
-    <row r="50" spans="3:6">
-      <c r="C50" s="20"/>
-    </row>
-    <row r="51" spans="3:6">
-      <c r="C51" s="20"/>
-    </row>
-    <row r="52" spans="3:6">
-      <c r="C52" s="20"/>
+      <c r="E50" s="22"/>
+      <c r="F50" s="20">
+        <f>SUM(F4:F44)</f>
+        <v>744.86000000000013</v>
+      </c>
+    </row>
+    <row r="51" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C51" s="17"/>
+    </row>
+    <row r="52" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C52" s="17"/>
+    </row>
+    <row r="53" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C53" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="A15:A40"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="A15:A41"/>
     <mergeCell ref="A1:XFD1"/>
     <mergeCell ref="A2:XFD2"/>
     <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="A42:A44"/>
     <mergeCell ref="A4:A14"/>
-    <mergeCell ref="D46:E46"/>
     <mergeCell ref="D47:E47"/>
     <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D49:E49"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C31" r:id="rId1" xr:uid="{FA2E55DE-ECAE-6445-87F1-B54591E30DA4}"/>
+    <hyperlink ref="C32" r:id="rId1" xr:uid="{FA2E55DE-ECAE-6445-87F1-B54591E30DA4}"/>
+    <hyperlink ref="C44" r:id="rId2" xr:uid="{CA335BAA-FF93-0A47-9CDF-0FB4A6B36B3D}"/>
+    <hyperlink ref="C43" r:id="rId3" xr:uid="{E7C3BE30-B6E5-EB4E-8B90-F29A21C973A4}"/>
+    <hyperlink ref="C42" r:id="rId4" xr:uid="{1E1F9281-82D6-C242-A112-53A21B5F9BCE}"/>
+    <hyperlink ref="C41" r:id="rId5" xr:uid="{C66EE2F8-BF3C-C846-9A80-FF9A19D87DE9}"/>
+    <hyperlink ref="C40" r:id="rId6" xr:uid="{E38C9639-83B0-014F-8E3F-78C401F32F57}"/>
+    <hyperlink ref="C4" r:id="rId7" xr:uid="{825E3CC7-FA2A-2346-B998-805428BA762B}"/>
+    <hyperlink ref="C5" r:id="rId8" xr:uid="{87F83EC2-841D-FD45-B99E-162D40F56AE6}"/>
+    <hyperlink ref="C6" r:id="rId9" xr:uid="{4B85D5CD-2BD6-3F4A-B9D4-224E7225BB74}"/>
+    <hyperlink ref="C7" r:id="rId10" xr:uid="{CA813F82-3883-6D44-A4EB-8ED6F61AA9B4}"/>
+    <hyperlink ref="C13" r:id="rId11" xr:uid="{20E26E4B-ED60-974D-BDFA-82BBADCE0646}"/>
+    <hyperlink ref="C14" r:id="rId12" xr:uid="{AE274035-47F5-E641-A62F-240675912254}"/>
+    <hyperlink ref="C8" r:id="rId13" xr:uid="{B7E9492A-02FB-A149-A296-51E94A08F87B}"/>
+    <hyperlink ref="C9" r:id="rId14" xr:uid="{2432B82C-4500-5A47-9260-94F2C40373A9}"/>
+    <hyperlink ref="C10" r:id="rId15" xr:uid="{9B14BA70-87C4-7E4B-860A-2C49A6B0C45A}"/>
+    <hyperlink ref="C11" r:id="rId16" xr:uid="{503F11E7-79F4-C049-9A4A-F3F1F583E8E3}"/>
+    <hyperlink ref="C12" r:id="rId17" xr:uid="{64D98538-5DAE-4046-BA92-3B3940B2B7C4}"/>
+    <hyperlink ref="C15" r:id="rId18" xr:uid="{ABC11CDE-5A22-D941-B546-C26DD9F5194A}"/>
+    <hyperlink ref="C16" r:id="rId19" xr:uid="{E6E3ED49-5C1F-FA48-8EB8-84FD2586566A}"/>
+    <hyperlink ref="C17" r:id="rId20" xr:uid="{D129AAB5-D9D9-1046-AB55-3E074718492C}"/>
+    <hyperlink ref="C18" r:id="rId21" xr:uid="{2A6EBF1D-79F9-8242-8B17-4F0C151D516B}"/>
+    <hyperlink ref="C20" r:id="rId22" xr:uid="{6F83249A-E522-C246-8AB1-BCE08A5022B5}"/>
+    <hyperlink ref="C21" r:id="rId23" xr:uid="{6D49712D-98CC-ED4A-A5BF-BC21C0BB9AEC}"/>
+    <hyperlink ref="C22" r:id="rId24" xr:uid="{CC15793E-763D-EE40-9380-F02077EC8229}"/>
+    <hyperlink ref="C23" r:id="rId25" xr:uid="{4B8362AE-335B-E648-ADC5-56DF4ED5F165}"/>
+    <hyperlink ref="C24" r:id="rId26" xr:uid="{7D2D6336-3D0D-E44F-8F0D-00EBB005DB8C}"/>
+    <hyperlink ref="C25" r:id="rId27" xr:uid="{15F4BF16-0AF9-AE41-AA48-2C26DCC5A7C6}"/>
+    <hyperlink ref="C26" r:id="rId28" xr:uid="{57737966-802E-0646-A6E1-E36AB9742C21}"/>
+    <hyperlink ref="C27" r:id="rId29" xr:uid="{55BE69BA-4054-5348-968D-F93D43E28C6C}"/>
+    <hyperlink ref="C28" r:id="rId30" xr:uid="{F0FF17A3-0D74-9F47-9876-8C6285FD7C05}"/>
+    <hyperlink ref="C29" r:id="rId31" xr:uid="{19E0C263-7E0A-294F-899F-4784208B3133}"/>
+    <hyperlink ref="C30" r:id="rId32" xr:uid="{E919DA59-7739-374B-BC29-DD4A6E7C5CC5}"/>
+    <hyperlink ref="C31" r:id="rId33" xr:uid="{9C3DE551-DA3A-5441-935A-2CE371E55050}"/>
+    <hyperlink ref="C33" r:id="rId34" xr:uid="{369671CA-381A-6843-9E05-FFB00418223F}"/>
+    <hyperlink ref="C34" r:id="rId35" xr:uid="{2B7A5A28-FA17-7540-AD79-2B649C9E0595}"/>
+    <hyperlink ref="C35" r:id="rId36" xr:uid="{8AD858E5-7E4E-A645-A531-AC3E80F4DD9D}"/>
+    <hyperlink ref="C36" r:id="rId37" xr:uid="{E25199AF-19F7-6A41-9C3B-2D6649D283A7}"/>
+    <hyperlink ref="C37" r:id="rId38" xr:uid="{DDFE35EE-F8F9-E848-B9A0-392F1D1D78A3}"/>
+    <hyperlink ref="C38" r:id="rId39" xr:uid="{71031FA6-3A21-2D46-A297-520F2376FDF0}"/>
+    <hyperlink ref="C39" r:id="rId40" xr:uid="{BBF81E69-4E71-CB44-9B45-F0D33D9117A3}"/>
+    <hyperlink ref="C19" r:id="rId41" xr:uid="{A1502C7A-4594-E14D-89C2-70452BCC7525}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="64" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId42"/>
 </worksheet>
 </file>
</xml_diff>